<commit_message>
Wording changes and new files for 2022
</commit_message>
<xml_diff>
--- a/health-outbreak/resources/caselist.xlsx
+++ b/health-outbreak/resources/caselist.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20389"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Disc_Public Health\Courses I teach\1st yr Infect Dis\2021\Assignments\Outbreak investigation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Disc_Public Health\Courses I teach\1st yr Infect Dis\2022\Assignment\Outbreak investigation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A9FC00-77F1-4415-9996-2B266DC30BD3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13250"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Q fever Adelaide uni" sheetId="1" r:id="rId1"/>
+    <sheet name="Q fever line list" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -375,7 +376,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-C09]dd\-mmm\-yy;@"/>
   </numFmts>
@@ -996,6 +997,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1031,6 +1049,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1206,11 +1241,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1280,7 +1315,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>44206</v>
+        <v>44571</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -1321,7 +1356,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>44216</v>
+        <v>44581</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -1365,7 +1400,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>44232</v>
+        <v>44597</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -1409,7 +1444,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>44246</v>
+        <v>44611</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
@@ -1450,7 +1485,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>44260</v>
+        <v>44625</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -1491,7 +1526,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>44271</v>
+        <v>44636</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
@@ -1532,7 +1567,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>44271</v>
+        <v>44636</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
@@ -1576,7 +1611,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>44276</v>
+        <v>44641</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
@@ -1617,7 +1652,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>44289</v>
+        <v>44654</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
@@ -1661,7 +1696,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>44326</v>
+        <v>44691</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
@@ -1702,7 +1737,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>44341</v>
+        <v>44706</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
@@ -1743,7 +1778,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>44343</v>
+        <v>44708</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
@@ -1787,7 +1822,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>44389</v>
+        <v>44754</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
@@ -1828,7 +1863,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>44405</v>
+        <v>44770</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
@@ -1872,7 +1907,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="7">
-        <v>44422</v>
+        <v>44787</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>13</v>
@@ -1912,7 +1947,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="7">
-        <v>44424</v>
+        <v>44789</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>13</v>
@@ -1954,7 +1989,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="7">
-        <v>44424</v>
+        <v>44789</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>13</v>
@@ -1998,7 +2033,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="7">
-        <v>44426</v>
+        <v>44791</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>13</v>
@@ -2040,7 +2075,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="7">
-        <v>44431</v>
+        <v>44796</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>13</v>
@@ -2082,7 +2117,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="7">
-        <v>44431</v>
+        <v>44796</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>13</v>
@@ -2124,7 +2159,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="7">
-        <v>44432</v>
+        <v>44797</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>13</v>
@@ -2166,7 +2201,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="7">
-        <v>44432</v>
+        <v>44797</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>13</v>
@@ -2208,7 +2243,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="7">
-        <v>44433</v>
+        <v>44798</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>13</v>
@@ -2252,7 +2287,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="7">
-        <v>44434</v>
+        <v>44799</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>13</v>
@@ -2294,7 +2329,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="7">
-        <v>44436</v>
+        <v>44801</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>13</v>

</xml_diff>